<commit_message>
Updated test framework to use simple evaluation on the best solution at the very end to negate floating point precision errors
</commit_message>
<xml_diff>
--- a/Report/Comparison.xlsx
+++ b/Report/Comparison.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812CCA19-C13E-4093-98FC-C459D453FF43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAE4067-60CA-4343-A36A-6F098DADA5EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="4740" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking Comparison" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,35 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -96,8 +120,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -165,7 +190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -501,32 +526,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -586,10 +585,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -600,30 +598,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -633,7 +624,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -665,21 +656,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -992,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,532 +1001,868 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
         <v>2</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>3</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>4</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>5</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>6</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <v>7</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="8">
         <v>8</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="8">
         <v>9</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="40" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="C4" s="51">
+        <v>0.31073964325877701</v>
+      </c>
+      <c r="D4" s="30">
+        <v>0.31073964325877701</v>
+      </c>
+      <c r="E4" s="30">
+        <v>0.31158313223226802</v>
+      </c>
+      <c r="F4" s="30">
+        <v>0.310940670751644</v>
+      </c>
+      <c r="G4" s="30">
+        <v>0.310985907763902</v>
+      </c>
+      <c r="H4" s="30">
+        <v>0.310940670751644</v>
+      </c>
+      <c r="I4" s="30">
+        <v>0.31434330034059499</v>
+      </c>
+      <c r="J4" s="30">
+        <v>0.310940670751644</v>
+      </c>
+      <c r="K4" s="30">
+        <v>0.310940670751644</v>
+      </c>
+      <c r="L4" s="30">
+        <v>0.31109880338463303</v>
+      </c>
+      <c r="M4" s="30">
+        <v>0.310940670751644</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="C5" s="51">
+        <v>0.45730754157659198</v>
+      </c>
+      <c r="D5" s="30">
+        <v>0.48622964398645901</v>
+      </c>
+      <c r="E5" s="30">
+        <v>0.455724859810611</v>
+      </c>
+      <c r="F5" s="30">
+        <v>0.45730754157659198</v>
+      </c>
+      <c r="G5" s="30">
+        <v>0.45572659653167802</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0.45731399792446398</v>
+      </c>
+      <c r="I5" s="30">
+        <v>0.48622964398645901</v>
+      </c>
+      <c r="J5" s="30">
+        <v>0.489180685906142</v>
+      </c>
+      <c r="K5" s="30">
+        <v>0.455724859810611</v>
+      </c>
+      <c r="L5" s="30">
+        <v>0.45572659653167802</v>
+      </c>
+      <c r="M5" s="30">
+        <v>0.48622820718767701</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="C6" s="51">
+        <v>1.3334859180927401</v>
+      </c>
+      <c r="D6" s="30">
+        <v>1.31220516993206</v>
+      </c>
+      <c r="E6" s="30">
+        <v>1.3414734541953099</v>
+      </c>
+      <c r="F6" s="30">
+        <v>1.2961317133994801</v>
+      </c>
+      <c r="G6" s="30">
+        <v>1.3233456620467201</v>
+      </c>
+      <c r="H6" s="30">
+        <v>1.3298645638762501</v>
+      </c>
+      <c r="I6" s="30">
+        <v>1.3311187284977499</v>
+      </c>
+      <c r="J6" s="30">
+        <v>1.32357531052316</v>
+      </c>
+      <c r="K6" s="30">
+        <v>1.3119296715553099</v>
+      </c>
+      <c r="L6" s="30">
+        <v>1.2845387681114599</v>
+      </c>
+      <c r="M6" s="53">
+        <v>1.33856109347562</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
         <v>2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>3</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>4</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>5</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="8">
         <v>6</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <v>7</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="8">
         <v>8</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="8">
         <v>9</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="40" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="C10" s="51">
+        <v>0.310985907763902</v>
+      </c>
+      <c r="D10" s="30">
+        <v>0.31073964325877701</v>
+      </c>
+      <c r="E10" s="30">
+        <v>0.310940670751644</v>
+      </c>
+      <c r="F10" s="30">
+        <v>0.31073964325877701</v>
+      </c>
+      <c r="G10" s="30">
+        <v>0.31010422036546897</v>
+      </c>
+      <c r="H10" s="30">
+        <v>0.313136856144478</v>
+      </c>
+      <c r="I10" s="30">
+        <v>0.31268539532370099</v>
+      </c>
+      <c r="J10" s="30">
+        <v>0.310940670751644</v>
+      </c>
+      <c r="K10" s="30">
+        <v>0.31085253887950798</v>
+      </c>
+      <c r="L10" s="30">
+        <v>0.310985907763902</v>
+      </c>
+      <c r="M10" s="30">
+        <v>0.31268539532370099</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="C11" s="51">
+        <v>0.45941534662612699</v>
+      </c>
+      <c r="D11" s="30">
+        <v>0.46725060240433802</v>
+      </c>
+      <c r="E11" s="30">
+        <v>0.47127944236660402</v>
+      </c>
+      <c r="F11" s="30">
+        <v>0.455724859810611</v>
+      </c>
+      <c r="G11" s="30">
+        <v>0.47533553689768598</v>
+      </c>
+      <c r="H11" s="30">
+        <v>0.45730580485552502</v>
+      </c>
+      <c r="I11" s="30">
+        <v>0.455724859810611</v>
+      </c>
+      <c r="J11" s="30">
+        <v>0.45730580485552502</v>
+      </c>
+      <c r="K11" s="30">
+        <v>0.47614145860188301</v>
+      </c>
+      <c r="L11" s="30">
+        <v>0.46725060240433802</v>
+      </c>
+      <c r="M11" s="30">
+        <v>0.48559632650307499</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="C12" s="52">
+        <v>1.78796800021146</v>
+      </c>
+      <c r="D12" s="53">
+        <v>1.71904901612176</v>
+      </c>
+      <c r="E12" s="53">
+        <v>1.6779223132026699</v>
+      </c>
+      <c r="F12" s="53">
+        <v>1.6723467915192201</v>
+      </c>
+      <c r="G12" s="53">
+        <v>1.7697008315581499</v>
+      </c>
+      <c r="H12" s="53">
+        <v>1.66079601490317</v>
+      </c>
+      <c r="I12" s="53">
+        <v>1.7088345752106699</v>
+      </c>
+      <c r="J12" s="53">
+        <v>1.7082697414919601</v>
+      </c>
+      <c r="K12" s="53">
+        <v>1.69032811225557</v>
+      </c>
+      <c r="L12" s="53">
+        <v>1.70400939187758</v>
+      </c>
+      <c r="M12" s="53">
+        <v>1.6361361385344699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
     </row>
     <row r="14" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="51" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="51" t="s">
+      <c r="E15" s="44"/>
+      <c r="F15" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="52"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="G15" s="44"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="53"/>
-      <c r="B16" s="25" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
-        <v>0</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
-        <v>1</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>0</v>
+      </c>
+      <c r="B17" s="13">
+        <f>IF(C10&lt;C4,0,IF(C10=C4,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="13">
+        <f>IF(C10&gt;C4,0,IF(C10=C4,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="13">
+        <f>IF(C11&lt;C5,0,IF(C11=C5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="13">
+        <f>IF(C11&gt;C5,0,IF(C11=C5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="9">
+        <f>IF(C12&lt;C6,0,IF(C12=C6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="10">
+        <f>IF(C12&gt;C6,0,IF(C12=C6,0.5,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
+        <v>1</v>
+      </c>
+      <c r="B18" s="13">
+        <f>IF(D10&lt;D4,0,IF(D10=D4,0.5,1))</f>
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="13">
+        <f>IF(D10&gt;D4,0,IF(D10=D4,0.5,1))</f>
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="13">
+        <f>IF(D11&lt;D5,0,IF(D11=D5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f>IF(D11&gt;D5,0,IF(D11=D5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="9">
+        <f>IF(D12&lt;D6,0,IF(D12=D6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <f>IF(D12&gt;D6,0,IF(D12=D6,0.5,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
         <v>2</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="22">
+      <c r="B19" s="13">
+        <f>IF(E10&lt;E4,0,IF(E10=E4,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="13">
+        <f>IF(E10&gt;E4,0,IF(E10=E4,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="13">
+        <f>IF(E11&lt;E5,0,IF(E11=E5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <f>IF(E11&gt;E5,0,IF(E11=E5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <f>IF(E12&lt;E6,0,IF(E12=E6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <f>IF(E12&gt;E6,0,IF(E12=E6,0.5,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
         <v>3</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="B20" s="13">
+        <f>IF(F10&lt;F4,0,IF(F10=F4,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="13">
+        <f>IF(F10&gt;F4,0,IF(F10=F4,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="13">
+        <f>IF(F11&lt;F5,0,IF(F11=F5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <f>IF(F11&gt;F5,0,IF(F11=F5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="9">
+        <f>IF(F12&lt;F6,0,IF(F12=F6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <f>IF(F12&gt;F6,0,IF(F12=F6,0.5,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
         <v>4</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
+      <c r="B21" s="13">
+        <f>IF(G10&lt;G4,0,IF(G10=G4,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="13">
+        <f>IF(G10&gt;G4,0,IF(G10=G4,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="13">
+        <f>IF(G11&lt;G5,0,IF(G11=G5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <f>IF(G11&gt;G5,0,IF(G11=G5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="9">
+        <f>IF(G12&lt;G6,0,IF(G12=G6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <f>IF(G12&gt;G6,0,IF(G12=G6,0.5,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
         <v>5</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="B22" s="13">
+        <f>IF(H10&lt;H4,0,IF(H10=H4,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="13">
+        <f>IF(H10&gt;H4,0,IF(H10=H4,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="13">
+        <f>IF(H11&lt;H5,0,IF(H11=H5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <f>IF(H11&gt;H5,0,IF(H11=H5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="9">
+        <f>IF(H12&lt;H6,0,IF(H12=H6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <f>IF(H12&gt;H6,0,IF(H12=H6,0.5,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
         <v>6</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
+      <c r="B23" s="13">
+        <f>IF(I10&lt;I4,0,IF(I10=I4,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="13">
+        <f>IF(I10&gt;I4,0,IF(I10=I4,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="13">
+        <f>IF(I11&lt;I5,0,IF(I11=I5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <f>IF(I11&gt;I5,0,IF(I11=I5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="9">
+        <f>IF(I12&lt;I6,0,IF(I12=I6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <f>IF(I12&gt;I6,0,IF(I12=I6,0.5,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
         <v>7</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="B24" s="13">
+        <f>IF(J10&lt;J4,0,IF(J10=J4,0.5,1))</f>
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="13">
+        <f>IF(J10&gt;J4,0,IF(J10=J4,0.5,1))</f>
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="13">
+        <f>IF(J11&lt;J5,0,IF(J11=J5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <f>IF(J11&gt;J5,0,IF(J11=J5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="9">
+        <f>IF(J12&lt;J6,0,IF(J12=J6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <f>IF(J12&gt;J6,0,IF(J12=J6,0.5,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15">
         <v>8</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
+      <c r="B25" s="13">
+        <f>IF(K10&lt;K4,0,IF(K10=K4,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="13">
+        <f>IF(K10&gt;K4,0,IF(K10=K4,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="13">
+        <f>IF(K11&lt;K5,0,IF(K11=K5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <f>IF(K11&gt;K5,0,IF(K11=K5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <f>IF(K12&lt;K6,0,IF(K12=K6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <f>IF(K12&gt;K6,0,IF(K12=K6,0.5,1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15">
         <v>9</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="3"/>
+      <c r="B26" s="13">
+        <f>IF(L10&lt;L4,0,IF(L10=L4,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="13">
+        <f>IF(L10&gt;L4,0,IF(L10=L4,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="13">
+        <f>IF(L11&lt;L5,0,IF(L11=L5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <f>IF(L11&gt;L5,0,IF(L11=L5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="9">
+        <f>IF(L12&lt;L6,0,IF(L12=L6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <f>IF(L12&gt;L6,0,IF(L12=L6,0.5,1))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23">
+      <c r="A27" s="16">
         <v>10</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="4"/>
+      <c r="B27" s="13">
+        <f>IF(M10&lt;M4,0,IF(M10=M4,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="13">
+        <f>IF(M10&gt;M4,0,IF(M10=M4,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="13">
+        <f>IF(M11&lt;M5,0,IF(M11=M5,0.5,1))</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <f>IF(M11&gt;M5,0,IF(M11=M5,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="9">
+        <f>IF(M12&lt;M6,0,IF(M12=M6,0.5,1))</f>
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <f>IF(M12&gt;M6,0,IF(M12=M6,0.5,1))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
     </row>
     <row r="29" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="4"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
+      <c r="B31" s="49" cm="1">
+        <f t="array" ref="B31">SUM(B17:B27+D17:D27+F17:F27)/(COUNT(B17:B27)+COUNT(D17:D27)+COUNT(F17:F27))</f>
+        <v>0.60606060606060608</v>
+      </c>
+      <c r="C31" s="50" cm="1">
+        <f t="array" ref="C31">SUM(C17:C27+E17:E27+G17:G27)/(COUNT(C17:C27)+COUNT(E17:E27)+COUNT(G17:G27))</f>
+        <v>0.39393939393939392</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1568,7 +1900,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
+      <c r="A2" s="23"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1576,7 +1908,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1584,245 +1916,245 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="23"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="54" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="54" t="s">
+      <c r="F10" s="47"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35" t="s">
+      <c r="D11" s="26"/>
+      <c r="E11" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="34"/>
-      <c r="I11" s="35" t="s">
+      <c r="H11" s="26"/>
+      <c r="I11" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="K11" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="32">
-        <v>0</v>
-      </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="E12" s="32">
-        <v>0</v>
-      </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="39"/>
-      <c r="I12" s="32">
-        <v>0</v>
-      </c>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
+      <c r="A12" s="24">
+        <v>0</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="E12" s="24">
+        <v>0</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="I12" s="24">
+        <v>0</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="32">
-        <v>1</v>
-      </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
-      <c r="E13" s="32">
-        <v>1</v>
-      </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
-      <c r="I13" s="32">
-        <v>1</v>
-      </c>
-      <c r="J13" s="38"/>
-      <c r="K13" s="39"/>
+      <c r="A13" s="24">
+        <v>1</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="E13" s="24">
+        <v>1</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31"/>
+      <c r="I13" s="24">
+        <v>1</v>
+      </c>
+      <c r="J13" s="30"/>
+      <c r="K13" s="31"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="32">
+      <c r="A14" s="24">
         <v>2</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="E14" s="32">
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
+      <c r="E14" s="24">
         <v>2</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="I14" s="32">
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
+      <c r="I14" s="24">
         <v>2</v>
       </c>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="31"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="32">
+      <c r="A15" s="24">
         <v>3</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-      <c r="E15" s="32">
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="E15" s="24">
         <v>3</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="I15" s="32">
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="I15" s="24">
         <v>3</v>
       </c>
-      <c r="J15" s="38"/>
-      <c r="K15" s="39"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+      <c r="A16" s="24">
         <v>4</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="E16" s="32">
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="E16" s="24">
         <v>4</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-      <c r="I16" s="32">
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
+      <c r="I16" s="24">
         <v>4</v>
       </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="31"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="32">
+      <c r="A17" s="24">
         <v>5</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="E17" s="32">
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
+      <c r="E17" s="24">
         <v>5</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39"/>
-      <c r="I17" s="32">
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
+      <c r="I17" s="24">
         <v>5</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="39"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="32">
+      <c r="A18" s="24">
         <v>6</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="E18" s="32">
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
+      <c r="E18" s="24">
         <v>6</v>
       </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="I18" s="32">
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="I18" s="24">
         <v>6</v>
       </c>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="31"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="32">
+      <c r="A19" s="24">
         <v>7</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
-      <c r="E19" s="32">
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="E19" s="24">
         <v>7</v>
       </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="I19" s="32">
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
+      <c r="I19" s="24">
         <v>7</v>
       </c>
-      <c r="J19" s="38"/>
-      <c r="K19" s="39"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="31"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="32">
+      <c r="A20" s="24">
         <v>8</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="39"/>
-      <c r="E20" s="32">
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="E20" s="24">
         <v>8</v>
       </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
-      <c r="I20" s="32">
+      <c r="F20" s="30"/>
+      <c r="G20" s="31"/>
+      <c r="I20" s="24">
         <v>8</v>
       </c>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="31"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="32">
+      <c r="A21" s="24">
         <v>9</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="39"/>
-      <c r="E21" s="32">
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="E21" s="24">
         <v>9</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
-      <c r="I21" s="32">
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
+      <c r="I21" s="24">
         <v>9</v>
       </c>
-      <c r="J21" s="38"/>
-      <c r="K21" s="39"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="33">
+      <c r="A22" s="25">
         <v>10</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="E22" s="33">
+      <c r="B22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="E22" s="25">
         <v>10</v>
       </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="41"/>
-      <c r="I22" s="33">
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="I22" s="25">
         <v>10</v>
       </c>
-      <c r="J22" s="40"/>
-      <c r="K22" s="41"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="33"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1836,9 +2168,9 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="I25" s="31"/>
+      <c r="A25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="I25" s="23"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1852,9 +2184,9 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="I28" s="31"/>
+      <c r="A28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="I28" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Redid the section of the report on the hyper heuristic as I've since changed how my hyperheuristic works. Also redid the results for the spreadsheets for the same reasons
</commit_message>
<xml_diff>
--- a/Report/Comparison.xlsx
+++ b/Report/Comparison.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAE4067-60CA-4343-A36A-6F098DADA5EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B692CC-F65A-4AD5-BB3D-E4A4EF60DD18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="Statistical Comparison" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -626,6 +627,11 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -671,11 +677,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -988,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
@@ -1001,38 +1002,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
     </row>
     <row r="2" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1076,13 +1077,13 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="45" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="36">
         <v>0.31073964325877701</v>
       </c>
       <c r="D4" s="30">
@@ -1117,11 +1118,11 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="36">
         <v>0.45730754157659198</v>
       </c>
       <c r="D5" s="30">
@@ -1156,11 +1157,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="36">
         <v>1.3334859180927401</v>
       </c>
       <c r="D6" s="30">
@@ -1190,7 +1191,7 @@
       <c r="L6" s="30">
         <v>1.2845387681114599</v>
       </c>
-      <c r="M6" s="53">
+      <c r="M6" s="38">
         <v>1.33856109347562</v>
       </c>
     </row>
@@ -1210,21 +1211,21 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -1268,13 +1269,13 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="45" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="36">
         <v>0.310985907763902</v>
       </c>
       <c r="D10" s="30">
@@ -1309,11 +1310,11 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="36">
         <v>0.45941534662612699</v>
       </c>
       <c r="D11" s="30">
@@ -1348,41 +1349,41 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="52">
+      <c r="C12" s="37">
         <v>1.78796800021146</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="38">
         <v>1.71904901612176</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="38">
         <v>1.6779223132026699</v>
       </c>
-      <c r="F12" s="53">
+      <c r="F12" s="38">
         <v>1.6723467915192201</v>
       </c>
-      <c r="G12" s="53">
+      <c r="G12" s="38">
         <v>1.7697008315581499</v>
       </c>
-      <c r="H12" s="53">
+      <c r="H12" s="38">
         <v>1.66079601490317</v>
       </c>
-      <c r="I12" s="53">
+      <c r="I12" s="38">
         <v>1.7088345752106699</v>
       </c>
-      <c r="J12" s="53">
+      <c r="J12" s="38">
         <v>1.7082697414919601</v>
       </c>
-      <c r="K12" s="53">
+      <c r="K12" s="38">
         <v>1.69032811225557</v>
       </c>
-      <c r="L12" s="53">
+      <c r="L12" s="38">
         <v>1.70400939187758</v>
       </c>
-      <c r="M12" s="53">
+      <c r="M12" s="38">
         <v>1.6361361385344699</v>
       </c>
     </row>
@@ -1390,38 +1391,38 @@
       <c r="A13" s="12"/>
     </row>
     <row r="14" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="43" t="s">
+      <c r="C15" s="49"/>
+      <c r="D15" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="43" t="s">
+      <c r="E15" s="49"/>
+      <c r="F15" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="44"/>
+      <c r="G15" s="49"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -1429,7 +1430,7 @@
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="18" t="s">
         <v>7</v>
       </c>
@@ -1789,21 +1790,21 @@
       <c r="M28" s="5"/>
     </row>
     <row r="29" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
@@ -1829,11 +1830,11 @@
       <c r="A31" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="49" cm="1">
+      <c r="B31" s="34" cm="1">
         <f t="array" ref="B31">SUM(B17:B27+D17:D27+F17:F27)/(COUNT(B17:B27)+COUNT(D17:D27)+COUNT(F17:F27))</f>
         <v>0.60606060606060608</v>
       </c>
-      <c r="C31" s="50" cm="1">
+      <c r="C31" s="35" cm="1">
         <f t="array" ref="C31">SUM(C17:C27+E17:E27+G17:G27)/(COUNT(C17:C27)+COUNT(E17:E27)+COUNT(G17:G27))</f>
         <v>0.39393939393939392</v>
       </c>
@@ -1848,21 +1849,21 @@
       <c r="M31" s="11"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1888,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B01021D-F22D-400F-A38F-8CC1F033904E}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,23 +1921,23 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="26"/>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="48"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="26"/>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="48"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="53"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">

</xml_diff>

<commit_message>
Improved section on delta evaluation and added statistical analysis spread sheet
</commit_message>
<xml_diff>
--- a/Report/Comparison.xlsx
+++ b/Report/Comparison.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B692CC-F65A-4AD5-BB3D-E4A4EF60DD18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565F9415-AA4B-4ADA-8C04-6A7AB899AA42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,6 @@
     <sheet name="Statistical Comparison" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>Domain</t>
   </si>
@@ -116,6 +115,24 @@
   <si>
     <t>PWP</t>
   </si>
+  <si>
+    <t>Wilcoxon Signed-Rank Test Calculator</t>
+  </si>
+  <si>
+    <t>The result is significant at p&lt;0.05</t>
+  </si>
+  <si>
+    <t>Two Tailed</t>
+  </si>
+  <si>
+    <t>The result is not significant at p&lt;0.05</t>
+  </si>
+  <si>
+    <t>The result is not significant at p &lt; 0.05</t>
+  </si>
+  <si>
+    <t>Added extra tests  (11 - 15) as some provided same values so wasn't able to calculate p-value in my statistical comparison (approved by Warren)</t>
+  </si>
 </sst>
 </file>
 
@@ -165,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,8 +207,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -580,13 +603,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -632,6 +690,11 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -668,6 +731,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,6 +747,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -713,6 +788,11 @@
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFF2CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -987,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,41 +1081,58 @@
     <col min="8" max="14" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-    </row>
-    <row r="2" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="1:25" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1072,12 +1169,23 @@
       <c r="L3" s="8">
         <v>9</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="41">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1113,12 +1221,23 @@
       <c r="L4" s="30">
         <v>0.31109880338463303</v>
       </c>
-      <c r="M4" s="30">
+      <c r="M4" s="42">
         <v>0.310940670751644</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="51"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1152,12 +1271,24 @@
       <c r="L5" s="30">
         <v>0.45572659653167802</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="42">
         <v>0.48622820718767701</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1191,11 +1322,23 @@
       <c r="L6" s="30">
         <v>1.2845387681114599</v>
       </c>
-      <c r="M6" s="38">
+      <c r="M6" s="43">
         <v>1.33856109347562</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+    </row>
+    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1209,25 +1352,49 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="41" t="s">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+    </row>
+    <row r="8" spans="1:25" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+    </row>
+    <row r="9" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
@@ -1264,12 +1431,24 @@
       <c r="L9" s="8">
         <v>9</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="41">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="50" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1305,12 +1484,24 @@
       <c r="L10" s="30">
         <v>0.310985907763902</v>
       </c>
-      <c r="M10" s="30">
+      <c r="M10" s="42">
         <v>0.31268539532370099</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1344,12 +1535,17 @@
       <c r="L11" s="30">
         <v>0.46725060240433802</v>
       </c>
-      <c r="M11" s="30">
+      <c r="M11" s="42">
         <v>0.48559632650307499</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="52"/>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1383,54 +1579,59 @@
       <c r="L12" s="38">
         <v>1.70400939187758</v>
       </c>
-      <c r="M12" s="38">
+      <c r="M12" s="43">
         <v>1.6361361385344699</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+    </row>
+    <row r="13" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
     </row>
-    <row r="14" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="43" t="s">
+    <row r="14" spans="1:25" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+    </row>
+    <row r="15" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="48" t="s">
+      <c r="C15" s="54"/>
+      <c r="D15" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="48" t="s">
+      <c r="E15" s="54"/>
+      <c r="F15" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="49"/>
+      <c r="G15" s="54"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
+    <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="55"/>
       <c r="B16" s="18" t="s">
         <v>7</v>
       </c>
@@ -1790,21 +1991,21 @@
       <c r="M28" s="5"/>
     </row>
     <row r="29" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
@@ -1849,21 +2050,21 @@
       <c r="M31" s="11"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="40"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1887,13 +2088,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B01021D-F22D-400F-A38F-8CC1F033904E}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1901,7 +2107,11 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
+      <c r="A2" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1909,35 +2119,43 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="57"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
+      <c r="J7" s="39"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="26"/>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="52"/>
-      <c r="G10" s="53"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="61"/>
       <c r="H10" s="26"/>
-      <c r="I10" s="51" t="s">
+      <c r="I10" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="52"/>
-      <c r="K10" s="53"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="61"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
@@ -1974,192 +2192,341 @@
       <c r="A12" s="24">
         <v>0</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
+      <c r="B12" s="30">
+        <v>0.31098590780000002</v>
+      </c>
+      <c r="C12" s="31">
+        <v>0.31073964329999998</v>
+      </c>
       <c r="E12" s="24">
         <v>0</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
+      <c r="F12" s="30">
+        <v>0.4594153466</v>
+      </c>
+      <c r="G12" s="31">
+        <v>0.45730754159999998</v>
+      </c>
       <c r="I12" s="24">
         <v>0</v>
       </c>
-      <c r="J12" s="30"/>
-      <c r="K12" s="31"/>
+      <c r="J12" s="30">
+        <v>1.7879680002</v>
+      </c>
+      <c r="K12" s="31">
+        <v>1.3334859181000001</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <v>1</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="30">
+        <v>0.31073964329999998</v>
+      </c>
+      <c r="C13" s="31">
+        <v>0.31073964329999998</v>
+      </c>
       <c r="E13" s="24">
         <v>1</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
+      <c r="F13" s="30">
+        <v>0.46725060239999999</v>
+      </c>
+      <c r="G13" s="31">
+        <v>0.48622964400000002</v>
+      </c>
       <c r="I13" s="24">
         <v>1</v>
       </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="31"/>
+      <c r="J13" s="30">
+        <v>1.7190490161</v>
+      </c>
+      <c r="K13" s="31">
+        <v>1.3122051698999999</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
         <v>2</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
+      <c r="B14" s="30">
+        <v>0.31094067079999999</v>
+      </c>
+      <c r="C14" s="31">
+        <v>0.3115831322</v>
+      </c>
       <c r="E14" s="24">
         <v>2</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
+      <c r="F14" s="30">
+        <v>0.47127944240000003</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.45572485979999999</v>
+      </c>
       <c r="I14" s="24">
         <v>2</v>
       </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="31"/>
+      <c r="J14" s="30">
+        <v>1.6779223132000001</v>
+      </c>
+      <c r="K14" s="31">
+        <v>1.3414734542</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
         <v>3</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
+      <c r="B15" s="30">
+        <v>0.31073964329999998</v>
+      </c>
+      <c r="C15" s="31">
+        <v>0.31094067079999999</v>
+      </c>
       <c r="E15" s="24">
         <v>3</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
+      <c r="F15" s="30">
+        <v>0.45572485979999999</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.45730754159999998</v>
+      </c>
       <c r="I15" s="24">
         <v>3</v>
       </c>
-      <c r="J15" s="30"/>
-      <c r="K15" s="31"/>
+      <c r="J15" s="30">
+        <v>1.6723467915000001</v>
+      </c>
+      <c r="K15" s="31">
+        <v>1.2961317134000001</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="24">
         <v>4</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
+      <c r="B16" s="30">
+        <v>0.31010422040000002</v>
+      </c>
+      <c r="C16" s="31">
+        <v>0.31098590780000002</v>
+      </c>
       <c r="E16" s="24">
         <v>4</v>
       </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
+      <c r="F16" s="30">
+        <v>0.47533553690000002</v>
+      </c>
+      <c r="G16" s="31">
+        <v>0.45572659650000003</v>
+      </c>
       <c r="I16" s="24">
         <v>4</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="31"/>
+      <c r="J16" s="30">
+        <v>1.7697008316</v>
+      </c>
+      <c r="K16" s="31">
+        <v>1.3233456619999999</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
         <v>5</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
+      <c r="B17" s="30">
+        <v>0.31313685610000003</v>
+      </c>
+      <c r="C17" s="31">
+        <v>0.31094067079999999</v>
+      </c>
       <c r="E17" s="24">
         <v>5</v>
       </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
+      <c r="F17" s="30">
+        <v>0.4573058049</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.45731399789999999</v>
+      </c>
       <c r="I17" s="24">
         <v>5</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="31"/>
+      <c r="J17" s="30">
+        <v>1.6607960149000001</v>
+      </c>
+      <c r="K17" s="31">
+        <v>1.3298645639</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>6</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
+      <c r="B18" s="30">
+        <v>0.3126853953</v>
+      </c>
+      <c r="C18" s="31">
+        <v>0.31434330030000002</v>
+      </c>
       <c r="E18" s="24">
         <v>6</v>
       </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
+      <c r="F18" s="30">
+        <v>0.45572485979999999</v>
+      </c>
+      <c r="G18" s="31">
+        <v>0.48622964400000002</v>
+      </c>
       <c r="I18" s="24">
         <v>6</v>
       </c>
-      <c r="J18" s="30"/>
-      <c r="K18" s="31"/>
+      <c r="J18" s="30">
+        <v>1.7088345752</v>
+      </c>
+      <c r="K18" s="31">
+        <v>1.3311187284999999</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
         <v>7</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
+      <c r="B19" s="30">
+        <v>0.31094067079999999</v>
+      </c>
+      <c r="C19" s="31">
+        <v>0.31094067079999999</v>
+      </c>
       <c r="E19" s="24">
         <v>7</v>
       </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
+      <c r="F19" s="30">
+        <v>0.4573058049</v>
+      </c>
+      <c r="G19" s="31">
+        <v>0.48918068590000002</v>
+      </c>
       <c r="I19" s="24">
         <v>7</v>
       </c>
-      <c r="J19" s="30"/>
-      <c r="K19" s="31"/>
+      <c r="J19" s="30">
+        <v>1.7082697415000001</v>
+      </c>
+      <c r="K19" s="31">
+        <v>1.3235753105000001</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
         <v>8</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="30">
+        <v>0.31085253889999998</v>
+      </c>
+      <c r="C20" s="31">
+        <v>0.31094067079999999</v>
+      </c>
       <c r="E20" s="24">
         <v>8</v>
       </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
+      <c r="F20" s="30">
+        <v>0.47614145860000001</v>
+      </c>
+      <c r="G20" s="31">
+        <v>0.45572485979999999</v>
+      </c>
       <c r="I20" s="24">
         <v>8</v>
       </c>
-      <c r="J20" s="30"/>
-      <c r="K20" s="31"/>
+      <c r="J20" s="30">
+        <v>1.6903281123</v>
+      </c>
+      <c r="K20" s="31">
+        <v>1.3119296716</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
         <v>9</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="30">
+        <v>0.31098590780000002</v>
+      </c>
+      <c r="C21" s="31">
+        <v>0.31109880340000001</v>
+      </c>
       <c r="E21" s="24">
         <v>9</v>
       </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
+      <c r="F21" s="30">
+        <v>0.46725060239999999</v>
+      </c>
+      <c r="G21" s="31">
+        <v>0.45572659650000003</v>
+      </c>
       <c r="I21" s="24">
         <v>9</v>
       </c>
-      <c r="J21" s="30"/>
-      <c r="K21" s="31"/>
+      <c r="J21" s="30">
+        <v>1.7040093918999999</v>
+      </c>
+      <c r="K21" s="31">
+        <v>1.2845387681</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25">
+      <c r="A22" s="24">
         <v>10</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="33"/>
+      <c r="B22" s="30">
+        <v>0.3126853953</v>
+      </c>
+      <c r="C22" s="31">
+        <v>0.31094067079999999</v>
+      </c>
       <c r="E22" s="25">
         <v>10</v>
       </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="F22" s="32">
+        <v>0.48559632650000001</v>
+      </c>
+      <c r="G22" s="33">
+        <v>0.48622820719999998</v>
+      </c>
       <c r="I22" s="25">
         <v>10</v>
       </c>
-      <c r="J22" s="32"/>
-      <c r="K22" s="33"/>
+      <c r="J22" s="32">
+        <v>1.6361361384999999</v>
+      </c>
+      <c r="K22" s="33">
+        <v>1.3385610935000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>11</v>
+      </c>
+      <c r="B23" s="30">
+        <v>0.31434329999999999</v>
+      </c>
+      <c r="C23" s="31">
+        <v>0.310940671</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
+      <c r="A24" s="24">
+        <v>12</v>
+      </c>
+      <c r="B24" s="30">
+        <v>0.31073964300000001</v>
+      </c>
+      <c r="C24" s="31">
+        <v>0.31085253899999998</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -2169,13 +2536,42 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="I25" s="23"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A25" s="24">
+        <v>13</v>
+      </c>
+      <c r="B25" s="30">
+        <v>0.32268511300000002</v>
+      </c>
+      <c r="C25" s="31">
+        <v>0.31010421999999999</v>
+      </c>
+      <c r="E25" s="23">
+        <v>0.92827999999999999</v>
+      </c>
+      <c r="I25" s="23">
+        <v>3.3800000000000002E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="24">
         <v>14</v>
+      </c>
+      <c r="B26" s="30">
+        <v>0.31085253899999998</v>
+      </c>
+      <c r="C26" s="31">
+        <v>0.31073964300000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <v>15</v>
+      </c>
+      <c r="B27" s="32">
+        <v>0.31073964300000001</v>
+      </c>
+      <c r="C27" s="33">
+        <v>0.31098590799999998</v>
       </c>
       <c r="E27" t="s">
         <v>14</v>
@@ -2185,15 +2581,143 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="I28" s="23"/>
+      <c r="E28" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="I28" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+    </row>
+    <row r="30" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="23">
+        <v>0.65993999999999997</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="11"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A10:C10"/>
+  <mergeCells count="9">
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="I10:K10"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>